<commit_message>
nmv 02 05 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.3 Padam Input Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136861D7-E63F-404F-AC57-BAAEA0D1F6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38F4858-F12F-4548-BB4E-0C6D4E5EBE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 5.3" sheetId="1" r:id="rId1"/>
@@ -3880,7 +3880,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4037,6 +4037,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4321,10 +4351,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2406" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1030" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N2478" sqref="N2478"/>
+      <selection pane="bottomLeft" activeCell="I1045" sqref="I1045:T1045"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -27238,37 +27268,37 @@
       <c r="U640" s="6"/>
       <c r="V640" s="42"/>
     </row>
-    <row r="641" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A641" s="6"/>
-      <c r="D641" s="19"/>
-      <c r="I641" s="39" t="s">
+    <row r="641" spans="1:22" s="55" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A641" s="54"/>
+      <c r="D641" s="56"/>
+      <c r="I641" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="J641" s="41">
+      <c r="J641" s="58">
         <v>14</v>
       </c>
-      <c r="K641" s="39">
+      <c r="K641" s="57">
         <f t="shared" si="27"/>
         <v>640</v>
       </c>
-      <c r="L641" s="39">
+      <c r="L641" s="57">
         <v>1</v>
       </c>
-      <c r="M641" s="39">
+      <c r="M641" s="57">
         <f t="shared" si="29"/>
         <v>151</v>
       </c>
-      <c r="N641" s="42" t="s">
+      <c r="N641" s="59" t="s">
         <v>421</v>
       </c>
-      <c r="O641" s="5"/>
-      <c r="P641" s="6"/>
-      <c r="Q641" s="6"/>
-      <c r="R641" s="6"/>
-      <c r="S641" s="6"/>
-      <c r="T641" s="6"/>
-      <c r="U641" s="6"/>
-      <c r="V641" s="42"/>
+      <c r="O641" s="60"/>
+      <c r="P641" s="54"/>
+      <c r="Q641" s="54"/>
+      <c r="R641" s="54"/>
+      <c r="S641" s="54"/>
+      <c r="T641" s="54"/>
+      <c r="U641" s="54"/>
+      <c r="V641" s="59"/>
     </row>
     <row r="642" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A642" s="6"/>
@@ -40375,35 +40405,35 @@
       <c r="V1044" s="42"/>
     </row>
     <row r="1045" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1045" s="39" t="s">
+      <c r="I1045" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="J1045" s="41">
+      <c r="J1045" s="62">
         <v>21</v>
       </c>
-      <c r="K1045" s="39">
+      <c r="K1045" s="61">
         <f t="shared" si="48"/>
         <v>1044</v>
       </c>
-      <c r="L1045" s="39">
+      <c r="L1045" s="61">
         <f t="shared" si="49"/>
         <v>50</v>
       </c>
-      <c r="M1045" s="39">
+      <c r="M1045" s="61">
         <f t="shared" si="50"/>
         <v>300</v>
       </c>
-      <c r="N1045" s="42" t="s">
+      <c r="N1045" s="63" t="s">
         <v>526</v>
       </c>
-      <c r="O1045" s="6" t="s">
+      <c r="O1045" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="P1045" s="6"/>
-      <c r="Q1045" s="6"/>
-      <c r="R1045" s="6"/>
-      <c r="S1045" s="6"/>
-      <c r="T1045" s="6"/>
+      <c r="P1045" s="10"/>
+      <c r="Q1045" s="10"/>
+      <c r="R1045" s="10"/>
+      <c r="S1045" s="10"/>
+      <c r="T1045" s="10"/>
       <c r="U1045" s="6"/>
       <c r="V1045" s="42" t="s">
         <v>1053</v>

</xml_diff>

<commit_message>
nmv 21 05 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.3 Padam Input Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21CB31F-8A50-4803-848A-A8D32741532D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BFE6EE-5753-4DE6-A553-7E1EDB2CE625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 5.3" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 5.3'!$C$1:$V$2478</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6398" uniqueCount="1217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6396" uniqueCount="1215">
   <si>
     <t>Passage</t>
   </si>
@@ -3363,9 +3363,6 @@
     <t>uqpaqdadhaqdityu#pa - dadha#t</t>
   </si>
   <si>
-    <t>utta#rAq ityut - taqrAH</t>
-  </si>
-  <si>
     <t>nAqkaqsadByaq iti# nAkaqsat - ByaqH</t>
   </si>
   <si>
@@ -3666,12 +3663,6 @@
     <t>3.13.11</t>
   </si>
   <si>
-    <t>NRE</t>
-  </si>
-  <si>
-    <t>anvanu</t>
-  </si>
-  <si>
     <t>1.20.11</t>
   </si>
   <si>
@@ -3679,6 +3670,9 @@
   </si>
   <si>
     <t>upA RutavyAH - elong</t>
+  </si>
+  <si>
+    <t>utta#rAq ityut - taqrAqH</t>
   </si>
 </sst>
 </file>
@@ -3881,7 +3875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4045,6 +4039,9 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4328,10 +4325,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2012" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1610" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1055" sqref="V1055"/>
+      <selection pane="bottomLeft" activeCell="A1624" sqref="A1624"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6683,7 +6680,7 @@
     </row>
     <row r="48" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A48" s="54" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="8"/>
@@ -22051,7 +22048,7 @@
     </row>
     <row r="490" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A490" s="6" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="D490" s="19"/>
       <c r="I490" s="39" t="s">
@@ -22085,7 +22082,7 @@
       <c r="T490" s="6"/>
       <c r="U490" s="6"/>
       <c r="V490" s="42" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="491" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -30684,7 +30681,7 @@
     </row>
     <row r="745" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A745" s="6" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="I745" s="39" t="s">
         <v>34</v>
@@ -30705,7 +30702,7 @@
         <v>255</v>
       </c>
       <c r="N745" s="42" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="O745" s="6" t="s">
         <v>68</v>
@@ -30719,7 +30716,7 @@
       <c r="T745" s="6"/>
       <c r="U745" s="6"/>
       <c r="V745" s="42" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="746" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42474,7 +42471,7 @@
         <v>364</v>
       </c>
       <c r="N1109" s="42" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="O1109" s="5"/>
       <c r="P1109" s="6" t="s">
@@ -42486,7 +42483,7 @@
       <c r="T1109" s="6"/>
       <c r="U1109" s="6"/>
       <c r="V1109" s="42" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="1110" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42609,10 +42606,10 @@
       <c r="Q1113" s="6"/>
       <c r="R1113" s="6"/>
       <c r="S1113" s="54" t="s">
-        <v>1215</v>
+        <v>1212</v>
       </c>
       <c r="T1113" s="6" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="U1113" s="6"/>
       <c r="V1113" s="42"/>
@@ -42964,7 +42961,7 @@
         <v>75</v>
       </c>
       <c r="T1124" s="6" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="U1124" s="6"/>
       <c r="V1124" s="42"/>
@@ -44675,7 +44672,7 @@
         <v>76</v>
       </c>
       <c r="T1176" s="6" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="U1176" s="6"/>
       <c r="V1176" s="42"/>
@@ -50380,7 +50377,7 @@
     </row>
     <row r="1352" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1352" s="6" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="C1352" s="34"/>
       <c r="I1352" s="39" t="s">
@@ -51211,10 +51208,10 @@
       <c r="Q1375" s="6"/>
       <c r="R1375" s="6"/>
       <c r="S1375" s="6" t="s">
+        <v>1201</v>
+      </c>
+      <c r="T1375" s="6" t="s">
         <v>1202</v>
-      </c>
-      <c r="T1375" s="6" t="s">
-        <v>1203</v>
       </c>
       <c r="U1375" s="6"/>
       <c r="V1375" s="42"/>
@@ -55441,10 +55438,10 @@
       <c r="Q1500" s="6"/>
       <c r="R1500" s="6"/>
       <c r="S1500" s="6" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="T1500" s="6" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="U1500" s="6"/>
       <c r="V1500" s="42"/>
@@ -55888,7 +55885,7 @@
     </row>
     <row r="1514" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1514" s="6" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="C1514" s="34"/>
       <c r="G1514" s="29"/>
@@ -55923,7 +55920,7 @@
       <c r="T1514" s="6"/>
       <c r="U1514" s="6"/>
       <c r="V1514" s="42" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="1515" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57776,7 +57773,7 @@
         <v>57</v>
       </c>
       <c r="N1571" s="42" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="O1571" s="6" t="s">
         <v>68</v>
@@ -58642,8 +58639,8 @@
       <c r="O1603" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="V1603" s="42" t="s">
-        <v>1111</v>
+      <c r="V1603" s="56" t="s">
+        <v>1214</v>
       </c>
     </row>
     <row r="1604" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58672,7 +58669,7 @@
         <v>68</v>
       </c>
       <c r="V1604" s="42" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="1605" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58800,7 +58797,7 @@
         <v>68</v>
       </c>
       <c r="V1609" s="42" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="1610" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58853,7 +58850,7 @@
         <v>68</v>
       </c>
       <c r="V1611" s="42" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="1612" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58975,7 +58972,7 @@
       </c>
       <c r="V1616" s="42"/>
     </row>
-    <row r="1617" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1617" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1617" s="39" t="s">
         <v>52</v>
       </c>
@@ -59004,7 +59001,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="1618" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1618" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1618" s="39" t="s">
         <v>52</v>
       </c>
@@ -59031,7 +59028,7 @@
       </c>
       <c r="V1618" s="42"/>
     </row>
-    <row r="1619" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1619" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1619" s="39" t="s">
         <v>52</v>
       </c>
@@ -59055,7 +59052,7 @@
       </c>
       <c r="V1619" s="42"/>
     </row>
-    <row r="1620" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1620" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1620" s="39" t="s">
         <v>52</v>
       </c>
@@ -59079,7 +59076,7 @@
       </c>
       <c r="V1620" s="42"/>
     </row>
-    <row r="1621" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1621" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1621" s="39" t="s">
         <v>52</v>
       </c>
@@ -59103,7 +59100,7 @@
       </c>
       <c r="V1621" s="42"/>
     </row>
-    <row r="1622" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1622" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1622" s="39" t="s">
         <v>52</v>
       </c>
@@ -59127,7 +59124,7 @@
       </c>
       <c r="V1622" s="42"/>
     </row>
-    <row r="1623" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1623" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1623" s="39" t="s">
         <v>52</v>
       </c>
@@ -59151,10 +59148,7 @@
       </c>
       <c r="V1623" s="42"/>
     </row>
-    <row r="1624" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1624" s="6" t="s">
-        <v>1213</v>
-      </c>
+    <row r="1624" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1624" s="39" t="s">
         <v>52</v>
       </c>
@@ -59179,12 +59173,9 @@
       <c r="O1624" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="U1624" s="1" t="s">
-        <v>1212</v>
-      </c>
       <c r="V1624" s="42"/>
     </row>
-    <row r="1625" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1625" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1625" s="39" t="s">
         <v>52</v>
       </c>
@@ -59208,7 +59199,7 @@
       </c>
       <c r="V1625" s="42"/>
     </row>
-    <row r="1626" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1626" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1626" s="39" t="s">
         <v>52</v>
       </c>
@@ -59237,7 +59228,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="1627" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1627" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1627" s="39" t="s">
         <v>52</v>
       </c>
@@ -59261,7 +59252,7 @@
       </c>
       <c r="V1627" s="42"/>
     </row>
-    <row r="1628" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1628" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1628" s="39" t="s">
         <v>52</v>
       </c>
@@ -59287,10 +59278,10 @@
         <v>68</v>
       </c>
       <c r="V1628" s="42" t="s">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="1629" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="1629" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1629" s="39" t="s">
         <v>52</v>
       </c>
@@ -59314,7 +59305,7 @@
       </c>
       <c r="V1629" s="42"/>
     </row>
-    <row r="1630" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1630" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1630" s="39" t="s">
         <v>52</v>
       </c>
@@ -59340,10 +59331,10 @@
         <v>72</v>
       </c>
       <c r="V1630" s="42" t="s">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="1631" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="1631" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1631" s="39" t="s">
         <v>52</v>
       </c>
@@ -59370,7 +59361,7 @@
       </c>
       <c r="V1631" s="42"/>
     </row>
-    <row r="1632" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1632" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1632" s="39" t="s">
         <v>52</v>
       </c>
@@ -59526,7 +59517,7 @@
         <v>68</v>
       </c>
       <c r="V1637" s="42" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="1638" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59709,7 +59700,7 @@
         <v>68</v>
       </c>
       <c r="V1644" s="42" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="1645" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59916,7 +59907,7 @@
         <v>68</v>
       </c>
       <c r="V1652" s="42" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="1653" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59993,7 +59984,7 @@
         <v>68</v>
       </c>
       <c r="V1655" s="42" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="1656" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60145,7 +60136,7 @@
         <v>68</v>
       </c>
       <c r="V1661" s="42" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="1662" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60558,7 +60549,7 @@
         <v>68</v>
       </c>
       <c r="V1677" s="42" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="1678" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60617,7 +60608,7 @@
         <v>68</v>
       </c>
       <c r="V1679" s="42" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1680" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61579,7 +61570,7 @@
         <v>68</v>
       </c>
       <c r="V1716" s="42" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="1717" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61632,7 +61623,7 @@
         <v>68</v>
       </c>
       <c r="V1718" s="42" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="1719" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61685,7 +61676,7 @@
         <v>68</v>
       </c>
       <c r="V1720" s="42" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="1721" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61791,7 +61782,7 @@
         <v>68</v>
       </c>
       <c r="V1724" s="42" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="1725" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61996,13 +61987,13 @@
         <v>218</v>
       </c>
       <c r="N1732" s="42" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="O1732" s="6" t="s">
         <v>68</v>
       </c>
       <c r="V1732" s="42" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="1733" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62055,7 +62046,7 @@
         <v>68</v>
       </c>
       <c r="V1734" s="42" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="1735" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62105,7 +62096,7 @@
         <v>222</v>
       </c>
       <c r="N1736" s="42" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="O1736" s="6" t="s">
         <v>68</v>
@@ -62114,7 +62105,7 @@
         <v>69</v>
       </c>
       <c r="V1736" s="42" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="1737" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62717,7 +62708,7 @@
         <v>68</v>
       </c>
       <c r="V1760" s="42" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="1761" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63431,7 +63422,7 @@
         <v>68</v>
       </c>
       <c r="V1789" s="42" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="1790" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64093,7 +64084,7 @@
         <v>68</v>
       </c>
       <c r="V1816" s="42" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1817" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64226,7 +64217,7 @@
         <v>68</v>
       </c>
       <c r="V1821" s="42" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1822" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64385,7 +64376,7 @@
         <v>68</v>
       </c>
       <c r="V1827" s="42" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1828" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64439,7 +64430,7 @@
         <v>68</v>
       </c>
       <c r="V1829" s="42" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="1830" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64549,7 +64540,7 @@
         <v>68</v>
       </c>
       <c r="V1833" s="42" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="1834" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64679,7 +64670,7 @@
         <v>68</v>
       </c>
       <c r="V1838" s="42" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1839" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64807,7 +64798,7 @@
         <v>68</v>
       </c>
       <c r="V1843" s="42" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="1844" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65129,7 +65120,7 @@
         <v>68</v>
       </c>
       <c r="V1856" s="42" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="1857" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65209,7 +65200,7 @@
         <v>68</v>
       </c>
       <c r="V1859" s="42" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="1860" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65382,7 +65373,7 @@
         <v>68</v>
       </c>
       <c r="V1866" s="42" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="1867" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65555,7 +65546,7 @@
         <v>68</v>
       </c>
       <c r="V1873" s="42" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="1874" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65608,7 +65599,7 @@
         <v>68</v>
       </c>
       <c r="V1875" s="42" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="1876" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65786,7 +65777,7 @@
         <v>68</v>
       </c>
       <c r="V1882" s="42" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="1883" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65866,7 +65857,7 @@
         <v>68</v>
       </c>
       <c r="V1885" s="42" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="1886" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66093,7 +66084,7 @@
         <v>68</v>
       </c>
       <c r="V1894" s="42" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="1895" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66146,7 +66137,7 @@
         <v>68</v>
       </c>
       <c r="V1896" s="42" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="1897" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66295,7 +66286,7 @@
         <v>68</v>
       </c>
       <c r="V1902" s="42" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="1903" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66425,7 +66416,7 @@
         <v>68</v>
       </c>
       <c r="V1907" s="42" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="1908" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66654,7 +66645,7 @@
         <v>68</v>
       </c>
       <c r="V1916" s="42" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="1917" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66683,7 +66674,7 @@
         <v>68</v>
       </c>
       <c r="V1917" s="42" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="1918" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66808,7 +66799,7 @@
         <v>68</v>
       </c>
       <c r="V1922" s="42" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="1923" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67283,7 +67274,7 @@
         <v>68</v>
       </c>
       <c r="V1941" s="42" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="1942" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67384,7 +67375,7 @@
         <v>68</v>
       </c>
       <c r="V1945" s="42" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="1946" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67536,7 +67527,7 @@
         <v>68</v>
       </c>
       <c r="V1951" s="42" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="1952" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67667,7 +67658,7 @@
         <v>107</v>
       </c>
       <c r="V1956" s="42" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="1957" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67696,7 +67687,7 @@
         <v>68</v>
       </c>
       <c r="V1957" s="42" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="1958" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67947,7 +67938,7 @@
         <v>68</v>
       </c>
       <c r="V1967" s="42" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="1968" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68397,7 +68388,7 @@
         <v>68</v>
       </c>
       <c r="V1985" s="42" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1986" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68474,7 +68465,7 @@
         <v>68</v>
       </c>
       <c r="V1988" s="42" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="1989" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68559,7 +68550,7 @@
         <v>69</v>
       </c>
       <c r="V1991" s="42" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="1992" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69068,7 +69059,7 @@
         <v>68</v>
       </c>
       <c r="V2011" s="42" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="2012" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69389,7 +69380,7 @@
         <v>68</v>
       </c>
       <c r="V2024" s="42" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="2025" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69589,7 +69580,7 @@
         <v>68</v>
       </c>
       <c r="V2032" s="42" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="2033" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69618,7 +69609,7 @@
         <v>68</v>
       </c>
       <c r="V2033" s="42" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="2034" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69671,7 +69662,7 @@
         <v>68</v>
       </c>
       <c r="V2035" s="42" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="2036" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69753,7 +69744,7 @@
         <v>68</v>
       </c>
       <c r="V2038" s="42" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="2039" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69806,7 +69797,7 @@
         <v>68</v>
       </c>
       <c r="V2040" s="42" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="2041" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70149,7 +70140,7 @@
         <v>68</v>
       </c>
       <c r="V2054" s="42" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="2055" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70202,7 +70193,7 @@
         <v>68</v>
       </c>
       <c r="V2056" s="42" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="2057" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70491,7 +70482,7 @@
         <v>68</v>
       </c>
       <c r="V2067" s="42" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="2068" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70691,7 +70682,7 @@
         <v>68</v>
       </c>
       <c r="V2075" s="42" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="2076" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71062,7 +71053,7 @@
         <v>68</v>
       </c>
       <c r="V2090" s="42" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="2091" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71525,7 +71516,7 @@
         <v>68</v>
       </c>
       <c r="V2109" s="42" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="2110" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71958,7 +71949,7 @@
         <v>68</v>
       </c>
       <c r="V2126" s="42" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="2127" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72458,7 +72449,7 @@
         <v>68</v>
       </c>
       <c r="V2146" s="42" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="2147" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72807,7 +72798,7 @@
         <v>68</v>
       </c>
       <c r="V2160" s="42" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="2161" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73103,7 +73094,7 @@
         <v>68</v>
       </c>
       <c r="V2172" s="42" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="2173" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73530,7 +73521,7 @@
     </row>
     <row r="2190" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2190" s="6" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
       <c r="I2190" s="39" t="s">
         <v>62</v>
@@ -73557,7 +73548,7 @@
         <v>69</v>
       </c>
       <c r="V2190" s="42" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="2191" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73584,7 +73575,7 @@
         <v>68</v>
       </c>
       <c r="V2191" s="42" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="2192" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73613,7 +73604,7 @@
         <v>68</v>
       </c>
       <c r="V2192" s="42" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="2193" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73990,7 +73981,7 @@
         <v>68</v>
       </c>
       <c r="V2207" s="42" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="2208" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74149,7 +74140,7 @@
         <v>68</v>
       </c>
       <c r="V2213" s="42" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="2214" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74178,7 +74169,7 @@
         <v>68</v>
       </c>
       <c r="V2214" s="42" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="2215" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74207,7 +74198,7 @@
         <v>68</v>
       </c>
       <c r="V2215" s="42" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="2216" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74599,7 +74590,7 @@
         <v>68</v>
       </c>
       <c r="V2231" s="42" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="2232" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75290,7 +75281,7 @@
         <v>68</v>
       </c>
       <c r="V2259" s="42" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="2260" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75343,7 +75334,7 @@
         <v>68</v>
       </c>
       <c r="V2261" s="42" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="2262" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75905,7 +75896,7 @@
         <v>68</v>
       </c>
       <c r="V2284" s="42" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="2285" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76928,7 +76919,7 @@
         <v>68</v>
       </c>
       <c r="V2324" s="42" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="2325" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77177,7 +77168,7 @@
         <v>68</v>
       </c>
       <c r="V2333" s="42" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="2334" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77230,7 +77221,7 @@
         <v>68</v>
       </c>
       <c r="V2335" s="42" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="2336" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77745,7 +77736,7 @@
         <v>68</v>
       </c>
       <c r="V2355" s="42" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="2356" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77823,7 +77814,7 @@
         <v>68</v>
       </c>
       <c r="V2358" s="42" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="2359" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77876,7 +77867,7 @@
         <v>68</v>
       </c>
       <c r="V2360" s="42" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="2361" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77905,7 +77896,7 @@
         <v>68</v>
       </c>
       <c r="V2361" s="42" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="2362" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78033,7 +78024,7 @@
         <v>69</v>
       </c>
       <c r="V2366" s="42" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="2367" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78060,7 +78051,7 @@
         <v>68</v>
       </c>
       <c r="V2367" s="42" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="2368" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78380,7 +78371,7 @@
         <v>68</v>
       </c>
       <c r="V2380" s="42" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="2381" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78457,7 +78448,7 @@
         <v>68</v>
       </c>
       <c r="V2383" s="42" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="2384" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78609,7 +78600,7 @@
         <v>68</v>
       </c>
       <c r="V2389" s="42" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="2390" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78710,7 +78701,7 @@
         <v>68</v>
       </c>
       <c r="V2393" s="42" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="2394" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79198,7 +79189,7 @@
         <v>68</v>
       </c>
       <c r="V2413" s="42" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="2414" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79373,7 +79364,7 @@
         <v>68</v>
       </c>
       <c r="V2419" s="42" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="2420" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79426,7 +79417,7 @@
         <v>68</v>
       </c>
       <c r="V2421" s="42" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="2422" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79623,7 +79614,7 @@
         <v>68</v>
       </c>
       <c r="V2429" s="42" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="2430" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79700,7 +79691,7 @@
         <v>68</v>
       </c>
       <c r="V2432" s="42" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="2433" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80049,7 +80040,7 @@
         <v>68</v>
       </c>
       <c r="V2446" s="42" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="2447" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80132,7 +80123,7 @@
         <v>68</v>
       </c>
       <c r="V2449" s="42" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="2450" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80317,10 +80308,10 @@
         <v>681</v>
       </c>
       <c r="S2456" s="6" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="T2456" s="6" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="V2456" s="42"/>
     </row>
@@ -80661,7 +80652,7 @@
         <v>68</v>
       </c>
       <c r="V2469" s="42" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="2470" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80884,7 +80875,7 @@
         <v>112</v>
       </c>
       <c r="N2478" s="42" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="O2478" s="6" t="s">
         <v>68</v>
@@ -80893,7 +80884,7 @@
         <v>69</v>
       </c>
       <c r="V2478" s="42" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nmv 24 07 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.3 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BFE6EE-5753-4DE6-A553-7E1EDB2CE625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6F172C-BDAC-454B-826A-0321595D214F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6396" uniqueCount="1215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6398" uniqueCount="1216">
   <si>
     <t>Passage</t>
   </si>
@@ -3673,6 +3673,9 @@
   </si>
   <si>
     <t>utta#rAq ityut - taqrAqH</t>
+  </si>
+  <si>
+    <t>N[s]</t>
   </si>
 </sst>
 </file>
@@ -3875,7 +3878,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4042,6 +4045,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4325,10 +4331,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2478"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1610" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1378" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A1624" sqref="A1624"/>
+      <selection pane="bottomLeft" activeCell="N1390" sqref="N1390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -51714,15 +51720,19 @@
         <f t="shared" si="65"/>
         <v>38</v>
       </c>
-      <c r="N1390" s="42" t="s">
+      <c r="N1390" s="57" t="s">
         <v>639</v>
       </c>
       <c r="O1390" s="5"/>
       <c r="P1390" s="6"/>
       <c r="Q1390" s="6"/>
       <c r="R1390" s="6"/>
-      <c r="S1390" s="6"/>
-      <c r="T1390" s="6"/>
+      <c r="S1390" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="T1390" s="54" t="s">
+        <v>1215</v>
+      </c>
       <c r="U1390" s="6"/>
       <c r="V1390" s="42"/>
     </row>
@@ -51746,7 +51756,7 @@
         <f t="shared" si="65"/>
         <v>39</v>
       </c>
-      <c r="N1391" s="42" t="s">
+      <c r="N1391" s="57" t="s">
         <v>640</v>
       </c>
       <c r="O1391" s="6"/>

</xml_diff>